<commit_message>
partlist updated to V0.5
Added new tab in excel with the partlist for the V0.5 board
</commit_message>
<xml_diff>
--- a/ConFLiCTuino.xlsx
+++ b/ConFLiCTuino.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="120" yWindow="96" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
-    <sheet name="ConFliCTuino 0.4" sheetId="1" r:id="rId1"/>
+    <sheet name="ConFliCTuino 0.5" sheetId="2" r:id="rId1"/>
+    <sheet name="ConFliCTuino 0.4" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="127">
   <si>
     <t>Qty</t>
   </si>
@@ -391,6 +392,21 @@
   </si>
   <si>
     <t>assemble with thermal grease and pads</t>
+  </si>
+  <si>
+    <t>A1-OUT1, A1-OUT2, A2-OUT1, A2-OUT2, FM, 1WIRE</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C7, C43, C51</t>
+  </si>
+  <si>
+    <t>22p</t>
+  </si>
+  <si>
+    <t>NPO-G0805 22P</t>
+  </si>
+  <si>
+    <t>R1, R31</t>
   </si>
 </sst>
 </file>
@@ -950,7 +966,14 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1250,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1312,6 +1335,775 @@
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="4">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="4">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="4">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="4">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="4">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="4.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="104" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2009,7 +2801,7 @@
     <mergeCell ref="H22:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>